<commit_message>
Prueba Cambio en el archivo
</commit_message>
<xml_diff>
--- a/Entrega1/ArmarComputador.xlsx
+++ b/Entrega1/ArmarComputador.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMS\Documents\Desarrollo_Software\Introduccion_Informatica\Prueba\mochila_camada7\mochila_camada7\Entrega1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D777EA2-30AF-453D-8248-53AE210FEAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA4F66A-C021-4FB6-9C45-0193CB8CFA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BA131171-F571-4BC3-B462-7FD4627A4180}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>GAMA BAJA</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>RTX 3070</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -185,14 +188,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{801C569A-E222-4091-8523-D326603DB678}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,133 +523,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>